<commit_message>
more post-class tweaks in (mostly) input files
</commit_message>
<xml_diff>
--- a/Code/Python/test.xlsx
+++ b/Code/Python/test.xlsx
@@ -75,8 +75,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,7 +350,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -359,9 +360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -380,7 +379,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2">
@@ -390,11 +389,11 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3">
@@ -404,11 +403,11 @@
         <v>3</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4">
@@ -418,7 +417,7 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <v>7</v>
+        <v>7.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>